<commit_message>
Atualizar especificação da API
</commit_message>
<xml_diff>
--- a/docs/Especificação da API.xlsx
+++ b/docs/Especificação da API.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djsla\OneDrive\Ambiente de Trabalho\picand-go\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LUÍS PEREIRA\GitHub\picand-go\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4118C8DF-81BB-4BEE-873C-6F10C3BDA622}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360067E4-488B-45AB-99D9-10C11ADB70EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="-120" windowWidth="19740" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="117">
   <si>
     <t>Registo</t>
   </si>
@@ -268,6 +268,123 @@
   </si>
   <si>
     <t>getByDriver</t>
+  </si>
+  <si>
+    <t>/api/users/accepted</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Rota padrão ao acessar API</t>
+  </si>
+  <si>
+    <t>Registar uma empresa</t>
+  </si>
+  <si>
+    <t>Registar um cliente</t>
+  </si>
+  <si>
+    <t>Registar um condutor</t>
+  </si>
+  <si>
+    <t>Registar um admin</t>
+  </si>
+  <si>
+    <t>Fazer login</t>
+  </si>
+  <si>
+    <t>Visualizar informações da conta</t>
+  </si>
+  <si>
+    <t>Obter empresas</t>
+  </si>
+  <si>
+    <t>Obter utilizadores não aceites</t>
+  </si>
+  <si>
+    <t>Obter utilizadores aceites</t>
+  </si>
+  <si>
+    <t>Editar dados do utilizadpr</t>
+  </si>
+  <si>
+    <t>Editar palavra-passe do utilizadpr</t>
+  </si>
+  <si>
+    <t>Editar foto do utilizador</t>
+  </si>
+  <si>
+    <t>Editar carta de condução do condutor</t>
+  </si>
+  <si>
+    <t>Aceitar utilizador</t>
+  </si>
+  <si>
+    <t>Definir utilizador como admin</t>
+  </si>
+  <si>
+    <t>Apagar utilizador</t>
+  </si>
+  <si>
+    <t>Remover utilizador de admin</t>
+  </si>
+  <si>
+    <t>Obter entregas do condutor</t>
+  </si>
+  <si>
+    <t>Aceitar entrega</t>
+  </si>
+  <si>
+    <t>Concluir entrega</t>
+  </si>
+  <si>
+    <t>Cancelar encomenda</t>
+  </si>
+  <si>
+    <t>Criar encomenda</t>
+  </si>
+  <si>
+    <t>Obter encomendas da empresa</t>
+  </si>
+  <si>
+    <t>Obter encomendas do utilizador</t>
+  </si>
+  <si>
+    <t>Criar produto</t>
+  </si>
+  <si>
+    <t>Editar dados do produto</t>
+  </si>
+  <si>
+    <t>Editar foto do produti</t>
+  </si>
+  <si>
+    <t>Apagar produto</t>
+  </si>
+  <si>
+    <t>Obter empresas pelo nome</t>
+  </si>
+  <si>
+    <t>Obter produtos da empresa com login</t>
+  </si>
+  <si>
+    <t>/api/orders/driver</t>
+  </si>
+  <si>
+    <t>/api/orders/not-accepted</t>
+  </si>
+  <si>
+    <t>Obter encomendas entregues do condutor</t>
+  </si>
+  <si>
+    <t>getNotAccepted</t>
+  </si>
+  <si>
+    <t>getFromDriver</t>
+  </si>
+  <si>
+    <t>getByAccepted</t>
   </si>
 </sst>
 </file>
@@ -379,11 +496,11 @@
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,8 +808,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1198A39D-FAF6-4CC2-BC9B-BD1DFBB184C3}" name="Tabela_Requisitos" displayName="Tabela_Requisitos" ref="A2:D39" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A2:D39" xr:uid="{FA7D6100-5CD1-494D-A60D-8E892EAEC05C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1198A39D-FAF6-4CC2-BC9B-BD1DFBB184C3}" name="Tabela_Requisitos" displayName="Tabela_Requisitos" ref="A2:D42" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A2:D42" xr:uid="{FA7D6100-5CD1-494D-A60D-8E892EAEC05C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3FC58B53-8DA1-4447-BCED-3625FD40251E}" name="RESTFull URL" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="3" xr3:uid="{BFBE8AC3-C050-4F78-8B7C-E36215B1671A}" name="HTTP Action" dataDxfId="5" totalsRowDxfId="4"/>
@@ -1000,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925233BC-DEF4-4153-A45F-C1645D7758F5}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1012,17 +1129,19 @@
     <col min="2" max="2" width="11.25" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="24.875" customWidth="1"/>
+    <col min="5" max="5" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1035,16 +1154,20 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1057,16 +1180,20 @@
       <c r="D4" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>71</v>
       </c>
@@ -1079,8 +1206,11 @@
       <c r="D6" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>74</v>
       </c>
@@ -1093,8 +1223,11 @@
       <c r="D7" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
@@ -1107,8 +1240,11 @@
       <c r="D8" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>72</v>
       </c>
@@ -1121,16 +1257,20 @@
       <c r="D9" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1143,16 +1283,20 @@
       <c r="D11" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1165,8 +1309,11 @@
       <c r="D13" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1179,10 +1326,13 @@
       <c r="D14" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>35</v>
@@ -1190,41 +1340,50 @@
       <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
+      <c r="D15" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>38</v>
@@ -1233,12 +1392,15 @@
         <v>42</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>38</v>
@@ -1247,12 +1409,15 @@
         <v>42</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>38</v>
@@ -1261,12 +1426,15 @@
         <v>42</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>38</v>
@@ -1275,12 +1443,15 @@
         <v>42</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>38</v>
@@ -1289,48 +1460,58 @@
         <v>42</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="E24" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>35</v>
@@ -1339,90 +1520,109 @@
         <v>43</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="E31" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>35</v>
@@ -1431,94 +1631,164 @@
         <v>44</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="E38" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="E40" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="E41" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>58</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="G2:G4">
-    <cfRule type="iconSet" priority="345">
+    <cfRule type="iconSet" priority="359">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1527,7 +1797,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="iconSet" priority="371">
+    <cfRule type="iconSet" priority="385">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1536,14 +1806,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="iconSet" priority="454">
+    <cfRule type="iconSet" priority="468">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="455">
+    <cfRule type="iconSet" priority="469">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1552,14 +1822,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="iconSet" priority="11">
+    <cfRule type="iconSet" priority="25">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="12">
+    <cfRule type="iconSet" priority="26">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1568,14 +1838,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="iconSet" priority="9">
+    <cfRule type="iconSet" priority="23">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="10">
+    <cfRule type="iconSet" priority="24">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1583,15 +1853,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="iconSet" priority="7">
+  <conditionalFormatting sqref="D25">
+    <cfRule type="iconSet" priority="21">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="8">
+    <cfRule type="iconSet" priority="22">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1599,15 +1869,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="iconSet" priority="5">
+  <conditionalFormatting sqref="D32">
+    <cfRule type="iconSet" priority="19">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="6">
+    <cfRule type="iconSet" priority="20">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1615,15 +1885,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="iconSet" priority="3">
+  <conditionalFormatting sqref="D39">
+    <cfRule type="iconSet" priority="17">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="4">
+    <cfRule type="iconSet" priority="18">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1632,14 +1902,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="iconSet" priority="1">
+    <cfRule type="iconSet" priority="15">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="16">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1648,7 +1918,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F6">
-    <cfRule type="iconSet" priority="456">
+    <cfRule type="iconSet" priority="470">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1657,7 +1927,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="iconSet" priority="458">
+    <cfRule type="iconSet" priority="472">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1665,8 +1935,120 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="iconSet" priority="13">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="14">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="iconSet" priority="11">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="12">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="iconSet" priority="9">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="10">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="iconSet" priority="7">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="8">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="6">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B32:B35 B37:B39 B4 B6:B9 B13:B23 B25:B30" xr:uid="{9C0731EB-549E-408A-A3E9-ABC1E65E8A6D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B13:B24 B40:B42 B4 B6:B9 B26:B31 B33:B38" xr:uid="{9C0731EB-549E-408A-A3E9-ABC1E65E8A6D}">
       <formula1>"GET,POST,PUT,PATCH,DELETE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>